<commit_message>
feat: update mind and tsp xmind
</commit_message>
<xml_diff>
--- a/___/table/technology-study-plan/Item/git仓库/参与开源作品.xlsx
+++ b/___/table/technology-study-plan/Item/git仓库/参与开源作品.xlsx
@@ -86,13 +86,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="mmm\ dd"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="mmm\ dd"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="ddd"/>
+    <numFmt numFmtId="177" formatCode="ddd"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -211,9 +211,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,10 +224,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,14 +245,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,7 +266,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,31 +286,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,11 +317,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -365,7 +365,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,7 +401,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,13 +431,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,19 +491,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,109 +527,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,6 +558,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,6 +601,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -597,15 +621,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -625,21 +640,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -655,76 +655,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -733,16 +733,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -751,46 +751,46 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -806,13 +806,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -854,7 +854,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -869,7 +869,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4517,7 +4517,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0d7740be-bbc6-49c9-a248-5fcbc5b6d0a1}</x14:id>
+          <x14:id>{030804bf-01f2-45d3-b857-b15220ced000}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4529,7 +4529,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bd2d603c-e445-4d93-ad8f-fb12e58cc4a4}</x14:id>
+          <x14:id>{fef2741a-bdf3-4c49-b015-a05772a447b0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4546,7 +4546,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0d7740be-bbc6-49c9-a248-5fcbc5b6d0a1}">
+          <x14:cfRule type="dataBar" id="{030804bf-01f2-45d3-b857-b15220ced000}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -4557,7 +4557,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{bd2d603c-e445-4d93-ad8f-fb12e58cc4a4}">
+          <x14:cfRule type="dataBar" id="{fef2741a-bdf3-4c49-b015-a05772a447b0}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -4640,7 +4640,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="12.8"/>
@@ -7486,7 +7486,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4655ec5a-14cf-4c23-af53-7d867c8523f2}</x14:id>
+          <x14:id>{69febcee-b77d-4390-852c-d560fc80b4a1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7498,7 +7498,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c9cb8e8f-3103-4457-b43c-97f55d4b13e6}</x14:id>
+          <x14:id>{2a0ffa01-becc-409f-912f-4f7d158e037e}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7515,7 +7515,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4655ec5a-14cf-4c23-af53-7d867c8523f2}">
+          <x14:cfRule type="dataBar" id="{69febcee-b77d-4390-852c-d560fc80b4a1}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -7526,7 +7526,7 @@
               <x14:axisColor indexed="65"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{c9cb8e8f-3103-4457-b43c-97f55d4b13e6}">
+          <x14:cfRule type="dataBar" id="{2a0ffa01-becc-409f-912f-4f7d158e037e}">
             <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>